<commit_message>
Added possibility to add balance
</commit_message>
<xml_diff>
--- a/changeLog.xlsx
+++ b/changeLog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>2014-27-01</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>Removida as colunas de valor e data para cadastro das despesas/receitas. Adicionado todos os meses e ano</t>
+  </si>
+  <si>
+    <t>Adicionada tabela com saldo</t>
+  </si>
+  <si>
+    <t>não</t>
   </si>
 </sst>
 </file>
@@ -81,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -384,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -466,6 +473,17 @@
       </c>
       <c r="C7" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>41761</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added posibility to add subordinates users
</commit_message>
<xml_diff>
--- a/changeLog.xlsx
+++ b/changeLog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
@@ -11,12 +11,12 @@
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>2014-27-01</t>
   </si>
@@ -58,13 +58,19 @@
   </si>
   <si>
     <t>Adicionado campo userMaster na tabela users</t>
+  </si>
+  <si>
+    <t>Adicionado indice na coluna email na tabela users (agora é campo único)</t>
+  </si>
+  <si>
+    <t>userType na table users agora é varchar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -185,7 +191,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -220,7 +225,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -396,26 +400,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3">
       <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -426,7 +430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -437,7 +441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -448,7 +452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -459,7 +463,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -470,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -481,7 +485,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3">
       <c r="A8" s="1">
         <v>41761</v>
       </c>
@@ -492,7 +496,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3">
       <c r="A9" s="1">
         <v>41676</v>
       </c>
@@ -503,7 +507,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3">
       <c r="A10" s="1">
         <v>41676</v>
       </c>
@@ -514,8 +518,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>41676</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>41676</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -523,24 +546,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Critical category exibition fix
</commit_message>
<xml_diff>
--- a/changeLog.xlsx
+++ b/changeLog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="20">
   <si>
     <t>2014-27-01</t>
   </si>
@@ -70,6 +70,12 @@
   </si>
   <si>
     <t>Alterado campo userId para userMaster na tabela de categorias varchar 255</t>
+  </si>
+  <si>
+    <t>Adicionado campo varchar ano na tabela cashflowcategories</t>
+  </si>
+  <si>
+    <t>não</t>
   </si>
 </sst>
 </file>
@@ -409,10 +415,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -579,6 +585,17 @@
       </c>
       <c r="C15" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>41832</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>